<commit_message>
Update Project Add ETL s_pm25_age_sex.py to project
</commit_message>
<xml_diff>
--- a/จังหวัด.xlsx
+++ b/จังหวัด.xlsx
@@ -5,17 +5,20 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chuwo\OneDrive\เอกสาร\Desktop\all_project\ETL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chuwo\OneDrive\เอกสาร\Desktop\all_project\Project_ETL_Data_From_REST_API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66BBB380-2AA7-4664-93E1-EBB9AF5A6F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF0D1F6-2EF1-478B-AD02-C38D4473A66C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B939F5D3-EDB3-4EE2-9051-D98FB9149003}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{B939F5D3-EDB3-4EE2-9051-D98FB9149003}"/>
   </bookViews>
   <sheets>
     <sheet name="end" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$C$79</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="80">
   <si>
     <t>no</t>
   </si>
@@ -183,9 +186,6 @@
     <t>หนองคาย</t>
   </si>
   <si>
-    <t xml:space="preserve">พระนครศรีอยุธยา	</t>
-  </si>
-  <si>
     <t>สตูล</t>
   </si>
   <si>
@@ -277,6 +277,9 @@
   </si>
   <si>
     <t>พระนครศรีอยุธยา</t>
+  </si>
+  <si>
+    <t>moph_id</t>
   </si>
 </sst>
 </file>
@@ -305,7 +308,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -315,6 +318,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -331,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -343,6 +352,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -679,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D384C069-F28F-4127-9AD3-ACA88CFB66F7}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -701,7 +711,7 @@
         <v>63</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
@@ -709,7 +719,7 @@
         <v>64</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
@@ -717,7 +727,7 @@
         <v>65</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
@@ -725,7 +735,7 @@
         <v>66</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
@@ -733,7 +743,7 @@
         <v>67</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
@@ -741,7 +751,7 @@
         <v>68</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
@@ -757,7 +767,7 @@
         <v>70</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.4">
@@ -765,7 +775,7 @@
         <v>71</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.4">
@@ -773,7 +783,7 @@
         <v>72</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.4">
@@ -781,7 +791,7 @@
         <v>73</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.4">
@@ -789,7 +799,7 @@
         <v>74</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.4">
@@ -797,7 +807,7 @@
         <v>75</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.4">
@@ -805,7 +815,7 @@
         <v>76</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.4">
@@ -813,7 +823,7 @@
         <v>77</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -823,10 +833,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBB5BF64-8930-428C-8988-4218A34C2906}">
-  <dimension ref="A1:B78"/>
+  <dimension ref="A1:C78"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B63" sqref="A60:B63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -834,631 +844,869 @@
     <col min="2" max="2" width="24.296875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C1" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+        <v>77</v>
+      </c>
+      <c r="C3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C4">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+        <v>76</v>
+      </c>
+      <c r="C5">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+        <v>75</v>
+      </c>
+      <c r="C6">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+        <v>74</v>
+      </c>
+      <c r="C7">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C8">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C9">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C10">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+        <v>73</v>
+      </c>
+      <c r="C11">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+        <v>72</v>
+      </c>
+      <c r="C12">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C13">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C14">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C15">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C16">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C17">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C18">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+        <v>71</v>
+      </c>
+      <c r="C19">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C20">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C21">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C22">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
+        <v>70</v>
+      </c>
+      <c r="C23">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C24">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C26">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C27">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
+        <v>69</v>
+      </c>
+      <c r="C28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C29">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
+        <v>68</v>
+      </c>
+      <c r="C30">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
+        <v>67</v>
+      </c>
+      <c r="C31">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C32">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C33">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
+        <v>66</v>
+      </c>
+      <c r="C34">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C36">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C37">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C38">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
+        <v>65</v>
+      </c>
+      <c r="C39">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C40">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C41">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.4">
+        <v>64</v>
+      </c>
+      <c r="C42">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C43">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C44">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C46">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C47">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C48">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C49">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C50">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.4">
+        <v>63</v>
+      </c>
+      <c r="C51">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C52">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.4">
+        <v>62</v>
+      </c>
+      <c r="C53">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C54">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C55">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C56">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C57">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C58">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C59">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C60">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C61">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C62">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.4">
+        <v>59</v>
+      </c>
+      <c r="C63">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.4">
+        <v>78</v>
+      </c>
+      <c r="C64">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.4">
+        <v>48</v>
+      </c>
+      <c r="C65">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.4">
+        <v>49</v>
+      </c>
+      <c r="C66">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.4">
+        <v>50</v>
+      </c>
+      <c r="C67">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.4">
+        <v>51</v>
+      </c>
+      <c r="C68">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.4">
+        <v>60</v>
+      </c>
+      <c r="C69">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C70">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.4">
+        <v>61</v>
+      </c>
+      <c r="C71">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.4">
+        <v>53</v>
+      </c>
+      <c r="C72">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.4">
+        <v>52</v>
+      </c>
+      <c r="C73">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A74">
         <v>73</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.4">
+        <v>54</v>
+      </c>
+      <c r="C74">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A75">
         <v>74</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.4">
+        <v>55</v>
+      </c>
+      <c r="C75">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A76">
         <v>75</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.4">
+        <v>56</v>
+      </c>
+      <c r="C76">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A77">
         <v>76</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.4">
+        <v>57</v>
+      </c>
+      <c r="C77">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A78">
         <v>77</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="C78">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C79" xr:uid="{EBB5BF64-8930-428C-8988-4218A34C2906}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C78">
+    <sortCondition ref="A1:A78"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>